<commit_message>
Inserido lógica de envio de e-mail  após a execução, e ajuste na estrutura do projeto.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\robo\Projetos UiPath\prj_HC_ContasMunicipais\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\robo\prj_HC_ContasMunicipais_SANASA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C031CF-F307-4275-A206-D745286152D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB08D2D-B8B9-45E4-BC88-2F1D68FEE8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14055" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -238,15 +238,9 @@
     <t>DownloadSanasaHVC_str_EmailDestinatario</t>
   </si>
   <si>
-    <t>DownloadSanasaHVC_Caminho_txt_UrlPortal</t>
-  </si>
-  <si>
     <t>Hospital Care/DownloadFaturas</t>
   </si>
   <si>
-    <t>Caminho onde está localizado o arquivo com o texto do corpo do email que será enviado aos destinatários</t>
-  </si>
-  <si>
     <t>DownloadSanasaHVC_PlanilhaTemplateRelatorio</t>
   </si>
   <si>
@@ -265,21 +259,12 @@
     <t xml:space="preserve">Email configurado para enviar os relatórios </t>
   </si>
   <si>
-    <t>DownloadSanasaHVC_Caminho_txt_CorpoEmail</t>
-  </si>
-  <si>
-    <t>Arquivo txt contendo a URL do portal SANASA</t>
-  </si>
-  <si>
     <t>PlanilhaTemplateRelatorio</t>
   </si>
   <si>
     <t>CaminhoPlanilhaRelatorioTemp</t>
   </si>
   <si>
-    <t>Caminho_txt_CorpoEmail</t>
-  </si>
-  <si>
     <t>EmailRemetente</t>
   </si>
   <si>
@@ -304,7 +289,13 @@
     <t>Servidor utilizado para envio do email</t>
   </si>
   <si>
-    <t>Sim</t>
+    <t>Caminho onde está localizado a planilha de controle de faturas</t>
+  </si>
+  <si>
+    <t>DownloadCPFLHVC_CaminhoPlanilhaFaturas</t>
+  </si>
+  <si>
+    <t>CaminhoPlanilhaFaturas</t>
   </si>
 </sst>
 </file>
@@ -704,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -766,7 +757,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -823,7 +814,7 @@
         <v>48</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>50</v>
@@ -889,13 +880,13 @@
     </row>
     <row r="20" spans="1:3" s="10" customFormat="1" ht="14.25" customHeight="1">
       <c r="A20" s="10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
@@ -1889,7 +1880,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1939,7 +1930,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>23</v>
@@ -3062,10 +3053,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3114,13 +3105,13 @@
     </row>
     <row r="2" spans="1:26" s="10" customFormat="1" ht="14.25" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>62</v>
@@ -3128,102 +3119,89 @@
     </row>
     <row r="3" spans="1:26" s="10" customFormat="1" ht="14.25" customHeight="1">
       <c r="A3" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>72</v>
-      </c>
       <c r="D3" s="10" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="10" customFormat="1" ht="14.25" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="10" customFormat="1" ht="14.25" customHeight="1">
       <c r="A5" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>75</v>
-      </c>
     </row>
-    <row r="6" spans="1:26" s="10" customFormat="1" ht="14.25" customHeight="1">
+    <row r="6" spans="1:26" ht="15" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>83</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="10" customFormat="1" ht="14.25" customHeight="1">
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="10" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1">
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>89</v>
-      </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4210,8 +4188,6 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajuste no wf de envio do email
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\robo\prj_HC_ContasMunicipais_SANASA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB08D2D-B8B9-45E4-BC88-2F1D68FEE8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713873E6-35DD-440E-8013-EF75D4C55DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14055" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3056,7 +3056,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Ajustes nos seletores no wf de download das faturas
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\robo\prj_HC_ContasMunicipais_SANASA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713873E6-35DD-440E-8013-EF75D4C55DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA6BBEE-A2BE-4781-8C84-F4134D7C2B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="14055" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -1879,8 +1879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1930,7 +1930,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>23</v>
@@ -3055,7 +3055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Ajustes na lógica do wf de abrir o navegador
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\robo\prj_HC_ContasMunicipais_SANASA\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\robo\Projetos UiPath\prj_HC_ContasMunicipais_SANASA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA6BBEE-A2BE-4781-8C84-F4134D7C2B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12B0F30-B35F-4831-B839-DBD64E50EB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -696,7 +696,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A18" sqref="A18:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1879,7 +1879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3055,7 +3055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add wf do banco de dados e ajustes de seletores
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\robo\Projetos UiPath\prj_HC_ContasMunicipais_SANASA\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\robo\prj_HC_ContasMunicipais_SANASA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12B0F30-B35F-4831-B839-DBD64E50EB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93C553F-3925-4131-A735-A8997600FE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
   <si>
     <t>Name</t>
   </si>
@@ -296,6 +296,12 @@
   </si>
   <si>
     <t>CaminhoPlanilhaFaturas</t>
+  </si>
+  <si>
+    <t>DownloadSanasaHVC_PathSQLITE</t>
+  </si>
+  <si>
+    <t>PathSQLITE</t>
   </si>
 </sst>
 </file>
@@ -3056,7 +3062,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3201,7 +3207,17 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Add anotação em variáveis e ajuste de seletores
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\robo\prj_HC_ContasMunicipais_SANASA\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\robo\Projetos UiPath\prj_HC_ContasMunicipais_SANASA\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93C553F-3925-4131-A735-A8997600FE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F595637D-1374-4994-8751-7B8873750985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -229,64 +229,22 @@
     <t>DownloadSanasaHVC_CredencialOrquestrator</t>
   </si>
   <si>
-    <t>Arquivo txt com indicando o caminho do download das faturas.</t>
-  </si>
-  <si>
-    <t>DownloadSanasaHVC_CaminhoDownload_txt_Faturas</t>
-  </si>
-  <si>
     <t>DownloadSanasaHVC_str_EmailDestinatario</t>
   </si>
   <si>
     <t>Hospital Care/DownloadFaturas</t>
   </si>
   <si>
-    <t>DownloadSanasaHVC_PlanilhaTemplateRelatorio</t>
-  </si>
-  <si>
-    <t>Caminho da planilha de relatório usada como template.</t>
-  </si>
-  <si>
-    <t>Caminho temporário da planilha de relatórios</t>
-  </si>
-  <si>
-    <t>DownloadSanasaHVC_CaminhoPlanilhaRelatorioTemp</t>
-  </si>
-  <si>
     <t>DownloadSanasaHVC_str_EmailRemetente</t>
   </si>
   <si>
     <t xml:space="preserve">Email configurado para enviar os relatórios </t>
   </si>
   <si>
-    <t>PlanilhaTemplateRelatorio</t>
-  </si>
-  <si>
-    <t>CaminhoPlanilhaRelatorioTemp</t>
-  </si>
-  <si>
     <t>EmailRemetente</t>
   </si>
   <si>
     <t>EmailDestinatarios</t>
-  </si>
-  <si>
-    <t>DownloadSanasaHVC_str_PortalEmail</t>
-  </si>
-  <si>
-    <t>PortalEmail</t>
-  </si>
-  <si>
-    <t>Porta utilizado para envio do email</t>
-  </si>
-  <si>
-    <t>DownloadSanasaHVC_ServerEmail</t>
-  </si>
-  <si>
-    <t>ServerEmail</t>
-  </si>
-  <si>
-    <t>Servidor utilizado para envio do email</t>
   </si>
   <si>
     <t>Caminho onde está localizado a planilha de controle de faturas</t>
@@ -702,7 +660,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:C18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -763,7 +721,7 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>30</v>
@@ -886,13 +844,13 @@
     </row>
     <row r="20" spans="1:3" s="10" customFormat="1" ht="14.25" customHeight="1">
       <c r="A20" s="10" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3059,10 +3017,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z995"/>
+  <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3111,113 +3069,48 @@
     </row>
     <row r="2" spans="1:26" s="10" customFormat="1" ht="14.25" customHeight="1">
       <c r="A2" s="10" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="10" customFormat="1" ht="14.25" customHeight="1">
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="D3" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>68</v>
-      </c>
     </row>
-    <row r="4" spans="1:26" s="10" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A4" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" s="10" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A5" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1">
-      <c r="A6" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>92</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4199,11 +4092,6 @@
     <row r="988" ht="14.25" customHeight="1"/>
     <row r="989" ht="14.25" customHeight="1"/>
     <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>